<commit_message>
Complete TIMSS 2015 Teacher Q
</commit_message>
<xml_diff>
--- a/RA/Nani_2022/T_15/T15_G4_5_Coding_explanation.xlsx
+++ b/RA/Nani_2022/T_15/T15_G4_5_Coding_explanation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Dropbox (UiO)\Nani\2022\T_15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416E07DA-9728-475A-B6B3-001EF43B4997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42B8E47-E220-4C16-82EE-2DE4848502C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16125" yWindow="5220" windowWidth="17280" windowHeight="9465" activeTab="1" xr2:uid="{746C5153-993A-4D34-9FB4-52770A3E65E7}"/>
+    <workbookView xWindow="9420" yWindow="1365" windowWidth="17280" windowHeight="9465" activeTab="1" xr2:uid="{746C5153-993A-4D34-9FB4-52770A3E65E7}"/>
   </bookViews>
   <sheets>
     <sheet name="1_G4_PV" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1212">
   <si>
     <t>IDCNTRY</t>
   </si>
@@ -3264,9 +3264,6 @@
     <t>SPDHour</t>
   </si>
   <si>
-    <t>(1=0) (2=1) (3=1) (4=3) (5=4)</t>
-  </si>
-  <si>
     <t>TIMSS compound variable: SEAS</t>
   </si>
   <si>
@@ -3604,6 +3601,75 @@
   </si>
   <si>
     <t>Number of students in Grade 4 class</t>
+  </si>
+  <si>
+    <t>SPrpLiv</t>
+  </si>
+  <si>
+    <t>SPrpBody</t>
+  </si>
+  <si>
+    <t>SPrpLife</t>
+  </si>
+  <si>
+    <t>SPrpPlan</t>
+  </si>
+  <si>
+    <t>SPrpFeat</t>
+  </si>
+  <si>
+    <t>SPrpComm</t>
+  </si>
+  <si>
+    <t>SPrpHum</t>
+  </si>
+  <si>
+    <t>SPrpMat</t>
+  </si>
+  <si>
+    <t>SPrpClas</t>
+  </si>
+  <si>
+    <t>SPrpMix</t>
+  </si>
+  <si>
+    <t>SPrpChg</t>
+  </si>
+  <si>
+    <t>SPrpEne</t>
+  </si>
+  <si>
+    <t>SPrpLigt</t>
+  </si>
+  <si>
+    <t>SPrpElec</t>
+  </si>
+  <si>
+    <t>SPrpMag</t>
+  </si>
+  <si>
+    <t>SPrpForc</t>
+  </si>
+  <si>
+    <t>SPrpLand</t>
+  </si>
+  <si>
+    <t>SPrpWate</t>
+  </si>
+  <si>
+    <t>SPrpWeat</t>
+  </si>
+  <si>
+    <t>SPrpFosl</t>
+  </si>
+  <si>
+    <t>SPrpSolr</t>
+  </si>
+  <si>
+    <t>SPrpMotn</t>
+  </si>
+  <si>
+    <t>SPrpReas</t>
   </si>
 </sst>
 </file>
@@ -5785,8 +5851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB5FA07-9B9D-4A17-BC77-5F8D8DD42BC3}">
   <dimension ref="A1:G305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159:C161"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="B266" sqref="B266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6166,7 +6232,7 @@
         <v>581</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="F25" s="7">
         <v>9</v>
@@ -6189,7 +6255,7 @@
         <v>582</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="F26" s="7">
         <v>9</v>
@@ -6212,7 +6278,7 @@
         <v>583</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="F27" s="7">
         <v>99</v>
@@ -7031,10 +7097,10 @@
         <v>337</v>
       </c>
       <c r="B63" s="11" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C63" s="12" t="s">
         <v>1105</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>1106</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>619</v>
@@ -7054,10 +7120,10 @@
         <v>338</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>620</v>
@@ -7077,10 +7143,10 @@
         <v>339</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>621</v>
@@ -7100,10 +7166,10 @@
         <v>340</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>622</v>
@@ -7123,10 +7189,10 @@
         <v>341</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>623</v>
@@ -7146,10 +7212,10 @@
         <v>342</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>624</v>
@@ -7169,10 +7235,10 @@
         <v>343</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>625</v>
@@ -7192,10 +7258,10 @@
         <v>344</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>626</v>
@@ -7215,10 +7281,10 @@
         <v>345</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>627</v>
@@ -7238,10 +7304,10 @@
         <v>346</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>628</v>
@@ -7261,10 +7327,10 @@
         <v>347</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>629</v>
@@ -7284,10 +7350,10 @@
         <v>348</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>630</v>
@@ -7307,10 +7373,10 @@
         <v>349</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>631</v>
@@ -7330,10 +7396,10 @@
         <v>350</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>632</v>
@@ -7698,7 +7764,7 @@
         <v>366</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>905</v>
@@ -7718,7 +7784,7 @@
         <v>367</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>906</v>
@@ -8124,10 +8190,10 @@
         <v>385</v>
       </c>
       <c r="B111" s="11" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C111" s="12" t="s">
         <v>1121</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>1122</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>667</v>
@@ -8147,10 +8213,10 @@
         <v>386</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>668</v>
@@ -8170,10 +8236,10 @@
         <v>387</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>669</v>
@@ -8193,10 +8259,10 @@
         <v>388</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>670</v>
@@ -8216,10 +8282,10 @@
         <v>389</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>671</v>
@@ -8239,10 +8305,10 @@
         <v>390</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>672</v>
@@ -8262,10 +8328,10 @@
         <v>391</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>673</v>
@@ -8285,10 +8351,10 @@
         <v>392</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>674</v>
@@ -8308,10 +8374,10 @@
         <v>393</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>675</v>
@@ -8656,7 +8722,7 @@
         <v>940</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>690</v>
@@ -8679,7 +8745,7 @@
         <v>940</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>691</v>
@@ -8702,7 +8768,7 @@
         <v>940</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>692</v>
@@ -9024,7 +9090,7 @@
         <v>973</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>706</v>
@@ -9113,7 +9179,7 @@
         <v>428</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>990</v>
@@ -9136,7 +9202,7 @@
         <v>429</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>991</v>
@@ -9159,7 +9225,7 @@
         <v>430</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>992</v>
@@ -9182,7 +9248,7 @@
         <v>431</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>993</v>
@@ -9205,7 +9271,7 @@
         <v>432</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>994</v>
@@ -9228,10 +9294,10 @@
         <v>433</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>715</v>
@@ -9251,10 +9317,10 @@
         <v>434</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>716</v>
@@ -9274,10 +9340,10 @@
         <v>435</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>717</v>
@@ -9481,16 +9547,16 @@
         <v>444</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>726</v>
       </c>
       <c r="E170" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F170" s="7">
         <v>9</v>
@@ -9504,16 +9570,16 @@
         <v>445</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C171" s="12" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>727</v>
       </c>
       <c r="E171" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F171" s="7">
         <v>9</v>
@@ -9527,16 +9593,16 @@
         <v>446</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>728</v>
       </c>
       <c r="E172" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F172" s="7">
         <v>9</v>
@@ -9550,16 +9616,16 @@
         <v>447</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D173" s="5" t="s">
         <v>729</v>
       </c>
       <c r="E173" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F173" s="7">
         <v>9</v>
@@ -9573,16 +9639,16 @@
         <v>448</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>730</v>
       </c>
       <c r="E174" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F174" s="7">
         <v>9</v>
@@ -9596,16 +9662,16 @@
         <v>449</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="D175" s="5" t="s">
         <v>731</v>
       </c>
       <c r="E175" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F175" s="7">
         <v>9</v>
@@ -9619,16 +9685,16 @@
         <v>450</v>
       </c>
       <c r="B176" s="11" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C176" s="12" t="s">
         <v>1144</v>
-      </c>
-      <c r="C176" s="12" t="s">
-        <v>1145</v>
       </c>
       <c r="D176" s="5" t="s">
         <v>732</v>
       </c>
       <c r="E176" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F176" s="7">
         <v>9</v>
@@ -9642,16 +9708,16 @@
         <v>451</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="D177" s="5" t="s">
         <v>733</v>
       </c>
       <c r="E177" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F177" s="7">
         <v>9</v>
@@ -9665,16 +9731,16 @@
         <v>452</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>734</v>
       </c>
       <c r="E178" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F178" s="7">
         <v>9</v>
@@ -9688,16 +9754,16 @@
         <v>453</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>735</v>
       </c>
       <c r="E179" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F179" s="7">
         <v>9</v>
@@ -9711,16 +9777,16 @@
         <v>454</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D180" s="5" t="s">
         <v>736</v>
       </c>
       <c r="E180" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F180" s="7">
         <v>9</v>
@@ -9734,16 +9800,16 @@
         <v>455</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C181" s="12" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="D181" s="5" t="s">
         <v>737</v>
       </c>
       <c r="E181" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F181" s="7">
         <v>9</v>
@@ -9757,16 +9823,16 @@
         <v>456</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D182" s="5" t="s">
         <v>738</v>
       </c>
       <c r="E182" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F182" s="7">
         <v>9</v>
@@ -9780,16 +9846,16 @@
         <v>457</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D183" s="5" t="s">
         <v>739</v>
       </c>
       <c r="E183" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F183" s="7">
         <v>9</v>
@@ -9803,16 +9869,16 @@
         <v>458</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D184" s="5" t="s">
         <v>740</v>
       </c>
       <c r="E184" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F184" s="7">
         <v>9</v>
@@ -9826,16 +9892,16 @@
         <v>459</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="D185" s="5" t="s">
         <v>741</v>
       </c>
       <c r="E185" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F185" s="7">
         <v>9</v>
@@ -9849,16 +9915,16 @@
         <v>460</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D186" s="5" t="s">
         <v>742</v>
       </c>
       <c r="E186" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F186" s="7">
         <v>9</v>
@@ -9915,10 +9981,10 @@
         <v>463</v>
       </c>
       <c r="B189" s="11" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C189" s="12" t="s">
         <v>1158</v>
-      </c>
-      <c r="C189" s="12" t="s">
-        <v>1159</v>
       </c>
       <c r="D189" s="5" t="s">
         <v>745</v>
@@ -9938,10 +10004,10 @@
         <v>464</v>
       </c>
       <c r="B190" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D190" s="5" t="s">
         <v>746</v>
@@ -9961,10 +10027,10 @@
         <v>465</v>
       </c>
       <c r="B191" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C191" s="14" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>747</v>
@@ -9984,10 +10050,10 @@
         <v>466</v>
       </c>
       <c r="B192" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>748</v>
@@ -10007,10 +10073,10 @@
         <v>467</v>
       </c>
       <c r="B193" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>749</v>
@@ -10030,10 +10096,10 @@
         <v>468</v>
       </c>
       <c r="B194" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="D194" s="5" t="s">
         <v>750</v>
@@ -10053,10 +10119,10 @@
         <v>469</v>
       </c>
       <c r="B195" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D195" s="5" t="s">
         <v>751</v>
@@ -10076,10 +10142,10 @@
         <v>470</v>
       </c>
       <c r="B196" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="D196" s="5" t="s">
         <v>752</v>
@@ -10099,10 +10165,10 @@
         <v>471</v>
       </c>
       <c r="B197" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="D197" s="5" t="s">
         <v>753</v>
@@ -10122,10 +10188,10 @@
         <v>472</v>
       </c>
       <c r="B198" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="D198" s="5" t="s">
         <v>754</v>
@@ -10562,7 +10628,7 @@
         <v>1029</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="D217" s="5" t="s">
         <v>773</v>
@@ -10585,7 +10651,7 @@
         <v>1029</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="D218" s="5" t="s">
         <v>774</v>
@@ -10608,7 +10674,7 @@
         <v>1029</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="D219" s="5" t="s">
         <v>775</v>
@@ -10631,7 +10697,7 @@
         <v>1029</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="D220" s="5" t="s">
         <v>776</v>
@@ -11295,10 +11361,10 @@
         <v>523</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C249" s="12" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="D249" s="5" t="s">
         <v>805</v>
@@ -11318,10 +11384,10 @@
         <v>524</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>1143</v>
+        <v>1172</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="D250" s="5" t="s">
         <v>806</v>
@@ -11341,10 +11407,10 @@
         <v>525</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>1143</v>
+        <v>1172</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D251" s="5" t="s">
         <v>807</v>
@@ -11557,7 +11623,7 @@
         <v>816</v>
       </c>
       <c r="E260" s="10" t="s">
-        <v>1076</v>
+        <v>995</v>
       </c>
       <c r="F260" s="7">
         <v>9</v>
@@ -11571,16 +11637,16 @@
         <v>535</v>
       </c>
       <c r="B261" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C261" s="14" t="s">
-        <v>1033</v>
+        <v>1189</v>
       </c>
       <c r="D261" s="5" t="s">
         <v>817</v>
       </c>
       <c r="E261" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F261" s="7">
         <v>9</v>
@@ -11594,16 +11660,16 @@
         <v>536</v>
       </c>
       <c r="B262" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C262" s="14" t="s">
-        <v>1034</v>
+        <v>1190</v>
       </c>
       <c r="D262" s="5" t="s">
         <v>818</v>
       </c>
       <c r="E262" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F262" s="7">
         <v>9</v>
@@ -11617,16 +11683,16 @@
         <v>537</v>
       </c>
       <c r="B263" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C263" s="14" t="s">
-        <v>1035</v>
+        <v>1191</v>
       </c>
       <c r="D263" s="5" t="s">
         <v>819</v>
       </c>
       <c r="E263" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F263" s="7">
         <v>9</v>
@@ -11640,16 +11706,16 @@
         <v>538</v>
       </c>
       <c r="B264" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C264" s="14" t="s">
-        <v>1036</v>
+        <v>1192</v>
       </c>
       <c r="D264" s="5" t="s">
         <v>820</v>
       </c>
       <c r="E264" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F264" s="7">
         <v>9</v>
@@ -11663,16 +11729,16 @@
         <v>539</v>
       </c>
       <c r="B265" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>1050</v>
+        <v>1193</v>
       </c>
       <c r="D265" s="5" t="s">
         <v>821</v>
       </c>
       <c r="E265" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F265" s="7">
         <v>9</v>
@@ -11686,16 +11752,16 @@
         <v>540</v>
       </c>
       <c r="B266" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C266" s="12" t="s">
-        <v>1051</v>
+        <v>1194</v>
       </c>
       <c r="D266" s="5" t="s">
         <v>822</v>
       </c>
       <c r="E266" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F266" s="7">
         <v>9</v>
@@ -11709,16 +11775,16 @@
         <v>541</v>
       </c>
       <c r="B267" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C267" s="14" t="s">
-        <v>1037</v>
+        <v>1195</v>
       </c>
       <c r="D267" s="5" t="s">
         <v>823</v>
       </c>
       <c r="E267" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F267" s="7">
         <v>9</v>
@@ -11732,16 +11798,16 @@
         <v>542</v>
       </c>
       <c r="B268" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C268" s="14" t="s">
-        <v>1038</v>
+        <v>1196</v>
       </c>
       <c r="D268" s="5" t="s">
         <v>824</v>
       </c>
       <c r="E268" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F268" s="7">
         <v>9</v>
@@ -11755,16 +11821,16 @@
         <v>543</v>
       </c>
       <c r="B269" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C269" s="14" t="s">
-        <v>1039</v>
+        <v>1197</v>
       </c>
       <c r="D269" s="5" t="s">
         <v>825</v>
       </c>
       <c r="E269" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F269" s="7">
         <v>9</v>
@@ -11778,16 +11844,16 @@
         <v>544</v>
       </c>
       <c r="B270" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C270" s="14" t="s">
-        <v>1040</v>
+        <v>1198</v>
       </c>
       <c r="D270" s="5" t="s">
         <v>826</v>
       </c>
       <c r="E270" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F270" s="7">
         <v>9</v>
@@ -11801,16 +11867,16 @@
         <v>545</v>
       </c>
       <c r="B271" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>1052</v>
+        <v>1199</v>
       </c>
       <c r="D271" s="5" t="s">
         <v>827</v>
       </c>
       <c r="E271" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F271" s="7">
         <v>9</v>
@@ -11824,16 +11890,16 @@
         <v>546</v>
       </c>
       <c r="B272" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C272" s="14" t="s">
-        <v>1042</v>
+        <v>1200</v>
       </c>
       <c r="D272" s="5" t="s">
         <v>828</v>
       </c>
       <c r="E272" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F272" s="7">
         <v>9</v>
@@ -11847,16 +11913,16 @@
         <v>547</v>
       </c>
       <c r="B273" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C273" s="14" t="s">
-        <v>1043</v>
+        <v>1201</v>
       </c>
       <c r="D273" s="5" t="s">
         <v>829</v>
       </c>
       <c r="E273" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F273" s="7">
         <v>9</v>
@@ -11870,16 +11936,16 @@
         <v>548</v>
       </c>
       <c r="B274" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C274" s="14" t="s">
-        <v>1044</v>
+        <v>1202</v>
       </c>
       <c r="D274" s="5" t="s">
         <v>830</v>
       </c>
       <c r="E274" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F274" s="7">
         <v>9</v>
@@ -11893,16 +11959,16 @@
         <v>549</v>
       </c>
       <c r="B275" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C275" s="14" t="s">
-        <v>1041</v>
+        <v>1203</v>
       </c>
       <c r="D275" s="5" t="s">
         <v>831</v>
       </c>
       <c r="E275" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F275" s="7">
         <v>9</v>
@@ -11916,16 +11982,16 @@
         <v>550</v>
       </c>
       <c r="B276" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C276" s="14" t="s">
-        <v>1045</v>
+        <v>1204</v>
       </c>
       <c r="D276" s="5" t="s">
         <v>832</v>
       </c>
       <c r="E276" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F276" s="7">
         <v>9</v>
@@ -11939,16 +12005,16 @@
         <v>551</v>
       </c>
       <c r="B277" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>1053</v>
+        <v>1205</v>
       </c>
       <c r="D277" s="5" t="s">
         <v>833</v>
       </c>
       <c r="E277" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F277" s="7">
         <v>9</v>
@@ -11962,16 +12028,16 @@
         <v>552</v>
       </c>
       <c r="B278" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C278" s="12" t="s">
-        <v>1054</v>
+        <v>1206</v>
       </c>
       <c r="D278" s="5" t="s">
         <v>834</v>
       </c>
       <c r="E278" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F278" s="7">
         <v>9</v>
@@ -11985,16 +12051,16 @@
         <v>553</v>
       </c>
       <c r="B279" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C279" s="12" t="s">
-        <v>1055</v>
+        <v>1207</v>
       </c>
       <c r="D279" s="5" t="s">
         <v>835</v>
       </c>
       <c r="E279" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F279" s="7">
         <v>9</v>
@@ -12008,16 +12074,16 @@
         <v>554</v>
       </c>
       <c r="B280" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C280" s="14" t="s">
-        <v>1046</v>
+        <v>1208</v>
       </c>
       <c r="D280" s="5" t="s">
         <v>836</v>
       </c>
       <c r="E280" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F280" s="7">
         <v>9</v>
@@ -12031,16 +12097,16 @@
         <v>555</v>
       </c>
       <c r="B281" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C281" s="14" t="s">
-        <v>1047</v>
+        <v>1209</v>
       </c>
       <c r="D281" s="5" t="s">
         <v>837</v>
       </c>
       <c r="E281" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F281" s="7">
         <v>9</v>
@@ -12054,16 +12120,16 @@
         <v>556</v>
       </c>
       <c r="B282" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C282" s="14" t="s">
-        <v>1048</v>
+        <v>1210</v>
       </c>
       <c r="D282" s="5" t="s">
         <v>838</v>
       </c>
       <c r="E282" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F282" s="7">
         <v>9</v>
@@ -12077,16 +12143,16 @@
         <v>557</v>
       </c>
       <c r="B283" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>1056</v>
+        <v>1211</v>
       </c>
       <c r="D283" s="5" t="s">
         <v>839</v>
       </c>
       <c r="E283" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F283" s="7">
         <v>9</v>
@@ -12100,10 +12166,10 @@
         <v>558</v>
       </c>
       <c r="B284" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C284" s="8" t="s">
         <v>1077</v>
-      </c>
-      <c r="C284" s="8" t="s">
-        <v>1078</v>
       </c>
       <c r="D284" s="5" t="s">
         <v>840</v>
@@ -12120,10 +12186,10 @@
         <v>559</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C285" s="8" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D285" s="5" t="s">
         <v>841</v>
@@ -12143,10 +12209,10 @@
         <v>560</v>
       </c>
       <c r="B286" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C286" s="4" t="s">
         <v>1080</v>
-      </c>
-      <c r="C286" s="4" t="s">
-        <v>1081</v>
       </c>
       <c r="D286" s="5" t="s">
         <v>842</v>
@@ -12163,10 +12229,10 @@
         <v>561</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D287" s="5" t="s">
         <v>843</v>
@@ -12186,10 +12252,10 @@
         <v>562</v>
       </c>
       <c r="B288" s="11" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="D288" s="5" t="s">
         <v>844</v>
@@ -12206,10 +12272,10 @@
         <v>563</v>
       </c>
       <c r="B289" s="11" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="D289" s="5" t="s">
         <v>845</v>
@@ -12229,10 +12295,10 @@
         <v>564</v>
       </c>
       <c r="B290" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C290" s="4" t="s">
         <v>1083</v>
-      </c>
-      <c r="C290" s="4" t="s">
-        <v>1084</v>
       </c>
       <c r="D290" s="5" t="s">
         <v>846</v>
@@ -12249,10 +12315,10 @@
         <v>565</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D291" s="5" t="s">
         <v>847</v>
@@ -12272,10 +12338,10 @@
         <v>566</v>
       </c>
       <c r="B292" s="11" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D292" s="5" t="s">
         <v>848</v>
@@ -12292,10 +12358,10 @@
         <v>567</v>
       </c>
       <c r="B293" s="11" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D293" s="5" t="s">
         <v>849</v>
@@ -12315,10 +12381,10 @@
         <v>568</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C294" s="4" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D294" s="5" t="s">
         <v>850</v>
@@ -12335,10 +12401,10 @@
         <v>569</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C295" s="4" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D295" s="5" t="s">
         <v>851</v>
@@ -12358,10 +12424,10 @@
         <v>570</v>
       </c>
       <c r="B296" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C296" s="4" t="s">
         <v>1088</v>
-      </c>
-      <c r="C296" s="4" t="s">
-        <v>1089</v>
       </c>
       <c r="D296" s="5" t="s">
         <v>852</v>
@@ -12378,10 +12444,10 @@
         <v>571</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D297" s="5" t="s">
         <v>853</v>
@@ -12401,16 +12467,16 @@
         <v>572</v>
       </c>
       <c r="B298" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C298" s="4" t="s">
         <v>1091</v>
-      </c>
-      <c r="C298" s="4" t="s">
-        <v>1092</v>
       </c>
       <c r="D298" s="5" t="s">
         <v>854</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F298" s="7">
         <v>9</v>
@@ -12424,16 +12490,16 @@
         <v>573</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C299" s="8" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D299" s="5" t="s">
         <v>855</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F299" s="7">
         <v>9</v>
@@ -12447,10 +12513,10 @@
         <v>574</v>
       </c>
       <c r="B300" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C300" s="4" t="s">
         <v>1093</v>
-      </c>
-      <c r="C300" s="4" t="s">
-        <v>1094</v>
       </c>
       <c r="D300" s="5" t="s">
         <v>856</v>
@@ -12467,10 +12533,10 @@
         <v>575</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D301" s="5" t="s">
         <v>857</v>
@@ -12487,10 +12553,10 @@
         <v>576</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D302" s="5" t="s">
         <v>858</v>
@@ -12507,10 +12573,10 @@
         <v>577</v>
       </c>
       <c r="B303" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C303" s="4" t="s">
         <v>1099</v>
-      </c>
-      <c r="C303" s="4" t="s">
-        <v>1100</v>
       </c>
       <c r="D303" s="5" t="s">
         <v>859</v>
@@ -12527,10 +12593,10 @@
         <v>578</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D304" s="5" t="s">
         <v>860</v>
@@ -12547,10 +12613,10 @@
         <v>579</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C305" s="4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D305" s="5" t="s">
         <v>861</v>

</xml_diff>